<commit_message>
Changed board text to match CC-SA wording, updated BOM
</commit_message>
<xml_diff>
--- a/leduinoBOM.xlsx
+++ b/leduinoBOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="leduinoBOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>Part</t>
   </si>
@@ -31,15 +31,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>R-US_R0805</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>RESISTOR, American symbol</t>
-  </si>
-  <si>
     <t>10uF</t>
   </si>
   <si>
@@ -76,9 +67,6 @@
     <t>10K</t>
   </si>
   <si>
-    <t>RN1</t>
-  </si>
-  <si>
     <t>4R-NEXB38V</t>
   </si>
   <si>
@@ -94,15 +82,9 @@
     <t>U1</t>
   </si>
   <si>
-    <t>MIC5219-5.0YM5</t>
-  </si>
-  <si>
     <t>V_REG_LDOSMD</t>
   </si>
   <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
     <t>Voltage Regulator LDO</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>Qty/board</t>
   </si>
   <si>
-    <t>Qty/panel</t>
-  </si>
-  <si>
     <t>U3-10</t>
   </si>
   <si>
@@ -145,9 +124,6 @@
     <t>CONN HEADR BRKWAY .100 40POS STR</t>
   </si>
   <si>
-    <t>S1, JP3</t>
-  </si>
-  <si>
     <t>Digikey Cost</t>
   </si>
   <si>
@@ -181,21 +157,9 @@
     <t>WM7736-ND</t>
   </si>
   <si>
-    <t>Cost/Panel</t>
-  </si>
-  <si>
-    <t>P10KACT-ND</t>
-  </si>
-  <si>
-    <t>R1-2</t>
-  </si>
-  <si>
     <t>Y9103CT-ND</t>
   </si>
   <si>
-    <t>576-2770-1-ND</t>
-  </si>
-  <si>
     <t>568-8366-5-ND</t>
   </si>
   <si>
@@ -205,9 +169,6 @@
     <t>MOSFET 2N-CH 60V 5A 8SO</t>
   </si>
   <si>
-    <t>C3-4</t>
-  </si>
-  <si>
     <t>C1-2</t>
   </si>
   <si>
@@ -251,6 +212,30 @@
   </si>
   <si>
     <t>BRAID</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>RN1-2</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>MIC39100-5.0WS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOT-223 </t>
+  </si>
+  <si>
+    <t>576-1173-ND</t>
+  </si>
+  <si>
+    <t>Cost/Board</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
 </sst>
 </file>
@@ -754,13 +739,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="16" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1104,10 +1092,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,12 +1105,12 @@
     <col min="4" max="4" width="35.140625" customWidth="1"/>
     <col min="5" max="5" width="48.140625" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1139,464 +1127,372 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>55</v>
+      <c r="I1" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G13" si="0">F2*6</f>
+      <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="I2" s="3">
+        <f>$F2*$H2</f>
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="J2" s="3">
-        <f t="shared" ref="J2:J16" si="1">G2*I2</f>
-        <v>4.08</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="G3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.1</v>
       </c>
-      <c r="J3" s="3">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I11" si="0">$F3*$H3</f>
+        <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="I4" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="2">
         <v>0.73</v>
       </c>
-      <c r="J4" s="3">
-        <f t="shared" si="1"/>
-        <v>4.38</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.54</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1.54</v>
-      </c>
-      <c r="J5" s="3">
-        <f t="shared" si="1"/>
-        <v>36.96</v>
+        <v>6.16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="2">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="J6" s="3">
-        <f t="shared" si="1"/>
-        <v>53.760000000000005</v>
+        <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="3">
-        <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <v>0.24</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3.01</v>
+      </c>
+      <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="J8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.72</v>
+        <v>3.01</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.66</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="2">
-        <v>3.01</v>
-      </c>
-      <c r="J9" s="3">
-        <f t="shared" si="1"/>
-        <v>18.059999999999999</v>
+        <v>1.66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2.36</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H10" s="1" t="s">
+        <v>2.36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="3">
+        <f>SUM(I2:I11)</f>
+        <v>27.679999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="2">
+        <v>15.3</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="2">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="J10" s="3">
-        <f t="shared" si="1"/>
-        <v>12.059999999999999</v>
-      </c>
+      <c r="G15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="2">
+        <v>14.93</v>
+      </c>
+      <c r="I15" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I11" s="2">
-        <v>2.36</v>
-      </c>
-      <c r="J11" s="3">
-        <f t="shared" si="1"/>
-        <v>14.16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12">
-        <v>8</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="J12" s="3">
-        <f t="shared" si="1"/>
-        <v>22.080000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I14" s="2">
-        <v>15.3</v>
-      </c>
-      <c r="J14" s="3">
-        <f t="shared" si="1"/>
-        <v>15.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I15" s="2">
-        <v>14.93</v>
-      </c>
-      <c r="J15" s="3">
-        <f>G15*I15</f>
-        <v>14.93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I16" s="2">
+      <c r="H16" s="2">
         <v>2.77</v>
       </c>
-      <c r="J16" s="3">
-        <f t="shared" si="1"/>
-        <v>2.77</v>
-      </c>
+      <c r="I16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>